<commit_message>
Add Dropdown for Code lists
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
+++ b/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/D073370/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC73031-DC2C-8D4A-B622-D763D9B130A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1388976-1EC6-E946-A6F2-0D8838C99508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13140" yWindow="2140" windowWidth="35020" windowHeight="23100" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="1" r:id="rId1"/>
+    <sheet name="Status" sheetId="2" r:id="rId2"/>
+    <sheet name="Priority" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Title</t>
   </si>
@@ -60,13 +62,34 @@
   </si>
   <si>
     <t>Example Document</t>
+  </si>
+  <si>
+    <t>Available Status</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Released</t>
+  </si>
+  <si>
+    <t>Available Priorities</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Very High</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,13 +105,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -100,32 +142,41 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -440,46 +491,148 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="48" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="106.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{60C2C633-DB22-5342-9E19-CECC27E7B0FA}">
+          <x14:formula1>
+            <xm:f>Status!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8BB50E1E-5B78-D548-8949-B820F38B4BC6}">
+          <x14:formula1>
+            <xm:f>Priority!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB49F8CB-3E12-D44F-9BCF-45137E5FF126}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D360D0CA-C5B6-E348-99AA-CF06125E1C9A}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Documents Excel Template
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
+++ b/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/D073370/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap.sharepoint.com/teams/Knowledge249/Shared Documents/Excel Import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1388976-1EC6-E946-A6F2-0D8838C99508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{A3C39EA5-A1D6-AD4A-8E2C-4716397A7C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDDEC835-A90D-2348-A212-9FBC678C1D3F}"/>
   <bookViews>
-    <workbookView xWindow="13140" yWindow="2140" windowWidth="35020" windowHeight="23100" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
+    <workbookView xWindow="-51200" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="1" r:id="rId1"/>
     <sheet name="Status" sheetId="2" r:id="rId2"/>
     <sheet name="Priority" sheetId="3" r:id="rId3"/>
+    <sheet name="Document Types" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,18 +39,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Title</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
     <t>Content</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Priority</t>
+    <t>Example Document One</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This is formatted content with HTML&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Example Document Two</t>
   </si>
   <si>
     <t>In Review</t>
@@ -58,16 +74,36 @@
     <t>High</t>
   </si>
   <si>
-    <t>&lt;p&gt;This is the formatted content of the document&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Example Document</t>
+    <t>This is unformatted plain text content without HTML</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">For detailed information on the creation of documents via spreadsheet, see </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SAP Help Portal.</t>
+    </r>
   </si>
   <si>
     <t>Available Status</t>
   </si>
   <si>
-    <t>In Progress</t>
+    <t>(default)</t>
   </si>
   <si>
     <t>Released</t>
@@ -76,20 +112,66 @@
     <t>Available Priorities</t>
   </si>
   <si>
+    <t>Very High</t>
+  </si>
+  <si>
     <t>Low</t>
   </si>
   <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Very High</t>
+    <t>Document Type</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>Available Document Types</t>
+  </si>
+  <si>
+    <t>Project Documentation</t>
+  </si>
+  <si>
+    <t>Not Assigned</t>
+  </si>
+  <si>
+    <t>Business Process Document</t>
+  </si>
+  <si>
+    <t>Solution Design Document</t>
+  </si>
+  <si>
+    <t>Fact Sheet</t>
+  </si>
+  <si>
+    <t>Functional Specification</t>
+  </si>
+  <si>
+    <t>Training Documentation</t>
+  </si>
+  <si>
+    <t>Technical Design Document</t>
+  </si>
+  <si>
+    <t>Configuration Guide</t>
+  </si>
+  <si>
+    <t>End-User Documentation</t>
+  </si>
+  <si>
+    <t>Interface Specification</t>
+  </si>
+  <si>
+    <t>[SAP Germany](https://sap.de)
+[SAP](https://sap.com)</t>
+  </si>
+  <si>
+    <t>[SAP](https://sap.com)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -113,8 +195,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,6 +219,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -157,11 +253,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -173,8 +270,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
@@ -189,6 +294,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -488,54 +597,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C19546E-5C87-714C-86D6-A993F68C66C3}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="106.83203125" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="44" customWidth="1"/>
+    <col min="6" max="6" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="C3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6:D6" r:id="rId1" display="For detailed information on the creation of documents via spreadsheet, see SAP Help Portal." xr:uid="{174D85B9-06DA-6342-A397-DF937288A6C3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{60C2C633-DB22-5342-9E19-CECC27E7B0FA}">
           <x14:formula1>
             <xm:f>Status!$A$2:$A$4</xm:f>
@@ -548,6 +702,12 @@
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1E751673-A5EC-E44D-9E48-703CCE71EEDE}">
+          <x14:formula1>
+            <xm:f>'Document Types'!$A$2:$A$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -556,83 +716,483 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB49F8CB-3E12-D44F-9BCF-45137E5FF126}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D360D0CA-C5B6-E348-99AA-CF06125E1C9A}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AAE950-B495-422A-8204-F5E1213B0FA9}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D360D0CA-C5B6-E348-99AA-CF06125E1C9A}">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d198314b-e946-45aa-aae0-63b36c0ef231" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BC4424C304B0C84BABB48D23FBFE0C27" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="47d1351a37322bfb439f27bbd0004be8">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d" xmlns:ns3="d198314b-e946-45aa-aae0-63b36c0ef231" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="33d4ea7c3c6a4a7f52d3013262c5b191" ns2:_="" ns3:_="">
+    <xsd:import namespace="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
+    <xsd:import namespace="d198314b-e946-45aa-aae0-63b36c0ef231"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c7b3fb9d-ee0a-40a8-bd42-4026b75186d8" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="23" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="24" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d198314b-e946-45aa-aae0-63b36c0ef231" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{087e4181-879a-4c77-88b0-7e72916adb31}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="d198314b-e946-45aa-aae0-63b36c0ef231">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0E3B64-8FFF-430D-A2EB-A1A771A45C34}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d198314b-e946-45aa-aae0-63b36c0ef231"/>
+    <ds:schemaRef ds:uri="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA75F62F-884B-498B-8B09-F712EECEEA19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
+    <ds:schemaRef ds:uri="d198314b-e946-45aa-aae0-63b36c0ef231"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB91C2F2-1F90-48E4-A244-DEC454B29DE6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjust Document Default Type
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
+++ b/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/D073370/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap.sharepoint.com/teams/Knowledge249/Shared Documents/Excel Import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1388976-1EC6-E946-A6F2-0D8838C99508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{A3C39EA5-A1D6-AD4A-8E2C-4716397A7C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5F69ED4-A383-4101-A162-5D99086D1391}"/>
   <bookViews>
-    <workbookView xWindow="13140" yWindow="2140" windowWidth="35020" windowHeight="23100" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
+    <workbookView xWindow="-51200" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="1" r:id="rId1"/>
     <sheet name="Status" sheetId="2" r:id="rId2"/>
     <sheet name="Priority" sheetId="3" r:id="rId3"/>
+    <sheet name="Document Types" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,18 +39,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Title</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Document Type</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
     <t>Content</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Priority</t>
+    <t>Example Document One</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>[SAP](https://sap.com)</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This is formatted content with HTML&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Example Document Two</t>
   </si>
   <si>
     <t>In Review</t>
@@ -58,16 +86,43 @@
     <t>High</t>
   </si>
   <si>
-    <t>&lt;p&gt;This is the formatted content of the document&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Example Document</t>
+    <t>End-User Documentation</t>
+  </si>
+  <si>
+    <t>[SAP Germany](https://sap.de)
+[SAP](https://sap.com)</t>
+  </si>
+  <si>
+    <t>This is unformatted plain text content without HTML</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">For detailed information on the creation of documents via spreadsheet, see </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SAP Help Portal.</t>
+    </r>
   </si>
   <si>
     <t>Available Status</t>
   </si>
   <si>
-    <t>In Progress</t>
+    <t>(default)</t>
   </si>
   <si>
     <t>Released</t>
@@ -76,20 +131,47 @@
     <t>Available Priorities</t>
   </si>
   <si>
+    <t>Very High</t>
+  </si>
+  <si>
     <t>Low</t>
   </si>
   <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Very High</t>
+    <t>Available Document Types</t>
+  </si>
+  <si>
+    <t>Project Documentation</t>
+  </si>
+  <si>
+    <t>Business Process Document</t>
+  </si>
+  <si>
+    <t>Solution Design Document</t>
+  </si>
+  <si>
+    <t>Functional Specification</t>
+  </si>
+  <si>
+    <t>Technical Design Document</t>
+  </si>
+  <si>
+    <t>Configuration Guide</t>
+  </si>
+  <si>
+    <t>Interface Specification</t>
+  </si>
+  <si>
+    <t>Training Documentation</t>
+  </si>
+  <si>
+    <t>Fact Sheet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -113,8 +195,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,6 +219,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -157,11 +253,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -173,8 +270,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
@@ -488,54 +593,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C19546E-5C87-714C-86D6-A993F68C66C3}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="106.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="24.375" customWidth="1"/>
+    <col min="5" max="5" width="44" customWidth="1"/>
+    <col min="6" max="6" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="32.25">
+      <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="C3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6:D6" r:id="rId1" display="For detailed information on the creation of documents via spreadsheet, see SAP Help Portal." xr:uid="{174D85B9-06DA-6342-A397-DF937288A6C3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{60C2C633-DB22-5342-9E19-CECC27E7B0FA}">
           <x14:formula1>
             <xm:f>Status!$A$2:$A$4</xm:f>
@@ -548,6 +698,12 @@
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1E751673-A5EC-E44D-9E48-703CCE71EEDE}">
+          <x14:formula1>
+            <xm:f>'Document Types'!$A$2:$A$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -556,35 +712,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB49F8CB-3E12-D44F-9BCF-45137E5FF126}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -595,44 +754,409 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D360D0CA-C5B6-E348-99AA-CF06125E1C9A}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AAE950-B495-422A-8204-F5E1213B0FA9}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <cols>
+    <col min="1" max="1" width="27.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d198314b-e946-45aa-aae0-63b36c0ef231" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BC4424C304B0C84BABB48D23FBFE0C27" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="47d1351a37322bfb439f27bbd0004be8">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d" xmlns:ns3="d198314b-e946-45aa-aae0-63b36c0ef231" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="33d4ea7c3c6a4a7f52d3013262c5b191" ns2:_="" ns3:_="">
+    <xsd:import namespace="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
+    <xsd:import namespace="d198314b-e946-45aa-aae0-63b36c0ef231"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c7b3fb9d-ee0a-40a8-bd42-4026b75186d8" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="23" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="24" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d198314b-e946-45aa-aae0-63b36c0ef231" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{087e4181-879a-4c77-88b0-7e72916adb31}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="d198314b-e946-45aa-aae0-63b36c0ef231">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB91C2F2-1F90-48E4-A244-DEC454B29DE6}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0E3B64-8FFF-430D-A2EB-A1A771A45C34}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA75F62F-884B-498B-8B09-F712EECEEA19}"/>
 </file>
</xml_diff>

<commit_message>
Add Owner Column to Excel Template
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
+++ b/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap.sharepoint.com/teams/Knowledge249/Shared Documents/Excel Import/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/D073879/Desktop/git/cloud-alm-api-examples/spreadsheet-examples/spreadsheet-documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{A3C39EA5-A1D6-AD4A-8E2C-4716397A7C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5F69ED4-A383-4101-A162-5D99086D1391}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7886D2DD-3B43-224E-ACA0-FC38A28ED4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
+    <workbookView xWindow="-38400" yWindow="-2580" windowWidth="38400" windowHeight="20280" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="1" r:id="rId1"/>
     <sheet name="Status" sheetId="2" r:id="rId2"/>
     <sheet name="Priority" sheetId="3" r:id="rId3"/>
-    <sheet name="Document Types" sheetId="4" r:id="rId4"/>
+    <sheet name="Types" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Title</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Priority</t>
-  </si>
-  <si>
-    <t>Document Type</t>
   </si>
   <si>
     <t>References</t>
@@ -137,9 +134,6 @@
     <t>Low</t>
   </si>
   <si>
-    <t>Available Document Types</t>
-  </si>
-  <si>
     <t>Project Documentation</t>
   </si>
   <si>
@@ -165,13 +159,28 @@
   </si>
   <si>
     <t>Fact Sheet</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>john.doe@sap.com</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Available Types</t>
+  </si>
+  <si>
+    <t>jane.doe@sap.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -258,7 +267,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -276,6 +285,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -593,23 +605,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C19546E-5C87-714C-86D6-A993F68C66C3}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="16.375" customWidth="1"/>
-    <col min="4" max="4" width="24.375" customWidth="1"/>
-    <col min="5" max="5" width="44" customWidth="1"/>
-    <col min="6" max="6" width="64" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="44" customWidth="1"/>
+    <col min="7" max="7" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -620,58 +633,67 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="16.5">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="32.25">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="7" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75">
-      <c r="A6" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -680,6 +702,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A6:D6" r:id="rId1" display="For detailed information on the creation of documents via spreadsheet, see SAP Help Portal." xr:uid="{174D85B9-06DA-6342-A397-DF937288A6C3}"/>
+    <hyperlink ref="E3" r:id="rId2" display="mailto:john.doe@sap.com" xr:uid="{1B87CAA8-28BE-D945-8C26-CFB2F21328D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -700,7 +723,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1E751673-A5EC-E44D-9E48-703CCE71EEDE}">
           <x14:formula1>
-            <xm:f>'Document Types'!$A$2:$A$12</xm:f>
+            <xm:f>Types!$A$2:$A$12</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
@@ -718,32 +741,32 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -760,37 +783,37 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.375" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -803,76 +826,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AAE950-B495-422A-8204-F5E1213B0FA9}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.875" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -881,28 +902,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d198314b-e946-45aa-aae0-63b36c0ef231" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BC4424C304B0C84BABB48D23FBFE0C27" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="47d1351a37322bfb439f27bbd0004be8">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d" xmlns:ns3="d198314b-e946-45aa-aae0-63b36c0ef231" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="33d4ea7c3c6a4a7f52d3013262c5b191" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BC4424C304B0C84BABB48D23FBFE0C27" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5926b03e82728d2d86cd579cef044969">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d" xmlns:ns3="d198314b-e946-45aa-aae0-63b36c0ef231" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b34dfbe06df4f742cab700692c9905" ns2:_="" ns3:_="">
     <xsd:import namespace="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
     <xsd:import namespace="d198314b-e946-45aa-aae0-63b36c0ef231"/>
     <xsd:element name="properties">
@@ -927,6 +928,7 @@
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1006,6 +1008,11 @@
     <xsd:element name="MediaServiceLocation" ma:index="24" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1149,14 +1156,45 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d198314b-e946-45aa-aae0-63b36c0ef231" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB91C2F2-1F90-48E4-A244-DEC454B29DE6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77130A33-8B41-4C6E-9374-3F37E025C758}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0E3B64-8FFF-430D-A2EB-A1A771A45C34}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0E3B64-8FFF-430D-A2EB-A1A771A45C34}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
+    <ds:schemaRef ds:uri="d198314b-e946-45aa-aae0-63b36c0ef231"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA75F62F-884B-498B-8B09-F712EECEEA19}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB91C2F2-1F90-48E4-A244-DEC454B29DE6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add Doc Type Test Document to Template
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
+++ b/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/D073879/Desktop/git/cloud-alm-api-examples/spreadsheet-examples/spreadsheet-documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7886D2DD-3B43-224E-ACA0-FC38A28ED4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{7886D2DD-3B43-224E-ACA0-FC38A28ED4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88277FCA-2022-467F-9825-D608A5A2A4E3}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-2580" windowWidth="38400" windowHeight="20280" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>Title</t>
   </si>
@@ -50,6 +50,12 @@
     <t>Priority</t>
   </si>
   <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
     <t>References</t>
   </si>
   <si>
@@ -68,6 +74,9 @@
     <t>Default</t>
   </si>
   <si>
+    <t>jane.doe@sap.com</t>
+  </si>
+  <si>
     <t>[SAP](https://sap.com)</t>
   </si>
   <si>
@@ -84,6 +93,9 @@
   </si>
   <si>
     <t>End-User Documentation</t>
+  </si>
+  <si>
+    <t>john.doe@sap.com</t>
   </si>
   <si>
     <t>[SAP Germany](https://sap.de)
@@ -134,6 +146,9 @@
     <t>Low</t>
   </si>
   <si>
+    <t>Available Types</t>
+  </si>
+  <si>
     <t>Project Documentation</t>
   </si>
   <si>
@@ -155,32 +170,20 @@
     <t>Interface Specification</t>
   </si>
   <si>
+    <t>Test Document</t>
+  </si>
+  <si>
     <t>Training Documentation</t>
   </si>
   <si>
     <t>Fact Sheet</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>john.doe@sap.com</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Available Types</t>
-  </si>
-  <si>
-    <t>jane.doe@sap.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -608,21 +611,21 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="24.375" customWidth="1"/>
+    <col min="5" max="5" width="18.125" customWidth="1"/>
     <col min="6" max="6" width="44" customWidth="1"/>
     <col min="7" max="7" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -633,67 +636,67 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17.100000000000001">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="33.950000000000003">
       <c r="A3" s="7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -723,7 +726,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1E751673-A5EC-E44D-9E48-703CCE71EEDE}">
           <x14:formula1>
-            <xm:f>Types!$A$2:$A$12</xm:f>
+            <xm:f>Types!$A$2:$A$13</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
@@ -741,32 +744,32 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -783,37 +786,37 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -824,76 +827,83 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AAE950-B495-422A-8204-F5E1213B0FA9}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" customWidth="1"/>
+    <col min="1" max="1" width="27.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -902,6 +912,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d198314b-e946-45aa-aae0-63b36c0ef231" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BC4424C304B0C84BABB48D23FBFE0C27" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5926b03e82728d2d86cd579cef044969">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d" xmlns:ns3="d198314b-e946-45aa-aae0-63b36c0ef231" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b34dfbe06df4f742cab700692c9905" ns2:_="" ns3:_="">
     <xsd:import namespace="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
@@ -1156,45 +1186,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d198314b-e946-45aa-aae0-63b36c0ef231" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB91C2F2-1F90-48E4-A244-DEC454B29DE6}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0E3B64-8FFF-430D-A2EB-A1A771A45C34}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77130A33-8B41-4C6E-9374-3F37E025C758}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0E3B64-8FFF-430D-A2EB-A1A771A45C34}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
-    <ds:schemaRef ds:uri="d198314b-e946-45aa-aae0-63b36c0ef231"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB91C2F2-1F90-48E4-A244-DEC454B29DE6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
rename training document to training material
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
+++ b/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/D073879/Desktop/git/cloud-alm-api-examples/spreadsheet-examples/spreadsheet-documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/D073370/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{7886D2DD-3B43-224E-ACA0-FC38A28ED4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88277FCA-2022-467F-9825-D608A5A2A4E3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAE7E5F-3FCA-5A47-8127-1D1495149939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-2580" windowWidth="38400" windowHeight="20280" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26780" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="1" r:id="rId1"/>
@@ -173,7 +173,7 @@
     <t>Test Document</t>
   </si>
   <si>
-    <t>Training Documentation</t>
+    <t>Training Material</t>
   </si>
   <si>
     <t>Fact Sheet</t>
@@ -183,7 +183,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -312,9 +312,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -352,7 +352,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -458,7 +458,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -600,7 +600,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -611,21 +611,21 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="16.375" customWidth="1"/>
-    <col min="4" max="4" width="24.375" customWidth="1"/>
-    <col min="5" max="5" width="18.125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
     <col min="6" max="6" width="44" customWidth="1"/>
     <col min="7" max="7" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -648,7 +648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17.100000000000001">
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -671,7 +671,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="33.950000000000003">
+    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
@@ -694,7 +694,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
@@ -744,17 +744,17 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -762,12 +762,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -786,27 +786,27 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.375" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -814,7 +814,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -830,20 +830,20 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.875" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -851,57 +851,57 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1187,13 +1187,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB91C2F2-1F90-48E4-A244-DEC454B29DE6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB91C2F2-1F90-48E4-A244-DEC454B29DE6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0E3B64-8FFF-430D-A2EB-A1A771A45C34}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0E3B64-8FFF-430D-A2EB-A1A771A45C34}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
+    <ds:schemaRef ds:uri="d198314b-e946-45aa-aae0-63b36c0ef231"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77130A33-8B41-4C6E-9374-3F37E025C758}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77130A33-8B41-4C6E-9374-3F37E025C758}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
+    <ds:schemaRef ds:uri="d198314b-e946-45aa-aae0-63b36c0ef231"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add new Doc Type "Note" to excel template
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
+++ b/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/D073370/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap.sharepoint.com/teams/Knowledge249/Shared Documents/Excel Import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAE7E5F-3FCA-5A47-8127-1D1495149939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{7886D2DD-3B43-224E-ACA0-FC38A28ED4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90F01222-5CAA-EF40-B8C2-952667C05875}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26780" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="47740" windowHeight="24440" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Title</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Fact Sheet</t>
+  </si>
+  <si>
+    <t>Note</t>
   </si>
 </sst>
 </file>
@@ -309,6 +312,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -611,7 +618,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -726,7 +733,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1E751673-A5EC-E44D-9E48-703CCE71EEDE}">
           <x14:formula1>
-            <xm:f>Types!$A$2:$A$13</xm:f>
+            <xm:f>Types!$A$2:$A$14</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
@@ -827,10 +834,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AAE950-B495-422A-8204-F5E1213B0FA9}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -904,6 +911,11 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1197,10 +1209,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0E3B64-8FFF-430D-A2EB-A1A771A45C34}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="d198314b-e946-45aa-aae0-63b36c0ef231"/>
     <ds:schemaRef ds:uri="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
-    <ds:schemaRef ds:uri="d198314b-e946-45aa-aae0-63b36c0ef231"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add new Doc Type - Job Documentation to Excel Template
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
+++ b/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap.sharepoint.com/teams/Knowledge249/Shared Documents/Excel Import/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap-my.sharepoint.com/personal/jim_grimm_sap_com/Documents/CALM/Excel FIles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{7886D2DD-3B43-224E-ACA0-FC38A28ED4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90F01222-5CAA-EF40-B8C2-952667C05875}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{7886D2DD-3B43-224E-ACA0-FC38A28ED4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7E73797-A225-4044-AF26-7FB0D44BA406}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="47740" windowHeight="24440" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
+    <workbookView xWindow="7240" yWindow="1860" windowWidth="34560" windowHeight="19980" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="1" r:id="rId1"/>
     <sheet name="Status" sheetId="2" r:id="rId2"/>
     <sheet name="Priority" sheetId="3" r:id="rId3"/>
     <sheet name="Types" sheetId="4" r:id="rId4"/>
+    <sheet name="Help Portal" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>Title</t>
   </si>
@@ -74,9 +75,6 @@
     <t>Default</t>
   </si>
   <si>
-    <t>jane.doe@sap.com</t>
-  </si>
-  <si>
     <t>[SAP](https://sap.com)</t>
   </si>
   <si>
@@ -93,9 +91,6 @@
   </si>
   <si>
     <t>End-User Documentation</t>
-  </si>
-  <si>
-    <t>john.doe@sap.com</t>
   </si>
   <si>
     <t>[SAP Germany](https://sap.de)
@@ -105,15 +100,71 @@
     <t>This is unformatted plain text content without HTML</t>
   </si>
   <si>
+    <t>Available Status</t>
+  </si>
+  <si>
+    <t>(default)</t>
+  </si>
+  <si>
+    <t>Released</t>
+  </si>
+  <si>
+    <t>Available Priorities</t>
+  </si>
+  <si>
+    <t>Very High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Available Types</t>
+  </si>
+  <si>
+    <t>Project Documentation</t>
+  </si>
+  <si>
+    <t>Business Process Document</t>
+  </si>
+  <si>
+    <t>Solution Design Document</t>
+  </si>
+  <si>
+    <t>Functional Specification</t>
+  </si>
+  <si>
+    <t>Technical Design Document</t>
+  </si>
+  <si>
+    <t>Configuration Guide</t>
+  </si>
+  <si>
+    <t>Interface Specification</t>
+  </si>
+  <si>
+    <t>Test Document</t>
+  </si>
+  <si>
+    <t>Training Material</t>
+  </si>
+  <si>
+    <t>Fact Sheet</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Job Documentation</t>
+  </si>
+  <si>
     <r>
       <rPr>
+        <u/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <rFont val="Calibri (Body)"/>
       </rPr>
-      <t xml:space="preserve">For detailed information on the creation of documents via spreadsheet, see </t>
+      <t>For detailed information on the creation of documents via spreadsheet, see</t>
     </r>
     <r>
       <rPr>
@@ -124,69 +175,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>SAP Help Portal.</t>
+      <t xml:space="preserve"> SAP Help Portal.</t>
     </r>
   </si>
   <si>
-    <t>Available Status</t>
-  </si>
-  <si>
-    <t>(default)</t>
-  </si>
-  <si>
-    <t>Released</t>
-  </si>
-  <si>
-    <t>Available Priorities</t>
-  </si>
-  <si>
-    <t>Very High</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Available Types</t>
-  </si>
-  <si>
-    <t>Project Documentation</t>
-  </si>
-  <si>
-    <t>Business Process Document</t>
-  </si>
-  <si>
-    <t>Solution Design Document</t>
-  </si>
-  <si>
-    <t>Functional Specification</t>
-  </si>
-  <si>
-    <t>Technical Design Document</t>
-  </si>
-  <si>
-    <t>Configuration Guide</t>
-  </si>
-  <si>
-    <t>Interface Specification</t>
-  </si>
-  <si>
-    <t>Test Document</t>
-  </si>
-  <si>
-    <t>Training Material</t>
-  </si>
-  <si>
-    <t>Fact Sheet</t>
-  </si>
-  <si>
-    <t>Note</t>
+    <t>jane.doe@sap.com</t>
+  </si>
+  <si>
+    <t>john.doe@sap.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -217,6 +220,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="5">
@@ -285,7 +294,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -294,6 +302,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -615,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C19546E-5C87-714C-86D6-A993F68C66C3}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -668,51 +679,43 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A6:D6" r:id="rId1" display="For detailed information on the creation of documents via spreadsheet, see SAP Help Portal." xr:uid="{174D85B9-06DA-6342-A397-DF937288A6C3}"/>
-    <hyperlink ref="E3" r:id="rId2" display="mailto:john.doe@sap.com" xr:uid="{1B87CAA8-28BE-D945-8C26-CFB2F21328D0}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{AD3020AE-47DB-104F-816E-B4B1CA52C568}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{045126C1-4C00-8144-814E-AFE3FC56189A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -731,9 +734,9 @@
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1E751673-A5EC-E44D-9E48-703CCE71EEDE}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4AC92AE6-FE61-A747-978E-796E22ADE355}">
           <x14:formula1>
-            <xm:f>Types!$A$2:$A$14</xm:f>
+            <xm:f>Types!$A$2:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
@@ -758,7 +761,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -766,17 +769,17 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -800,17 +803,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -818,12 +821,12 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -834,10 +837,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AAE950-B495-422A-8204-F5E1213B0FA9}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -847,7 +850,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -855,67 +858,72 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -923,27 +931,43 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99E68E23-2182-C74E-B87D-508B5DC0516E}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A4:H4"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:H4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" display="SAP Help Portal." xr:uid="{1CC217CD-20DC-B140-91CC-CE0A2AD9EBC2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d198314b-e946-45aa-aae0-63b36c0ef231" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BC4424C304B0C84BABB48D23FBFE0C27" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5926b03e82728d2d86cd579cef044969">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d" xmlns:ns3="d198314b-e946-45aa-aae0-63b36c0ef231" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b34dfbe06df4f742cab700692c9905" ns2:_="" ns3:_="">
     <xsd:import namespace="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
@@ -1198,32 +1222,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d198314b-e946-45aa-aae0-63b36c0ef231" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB91C2F2-1F90-48E4-A244-DEC454B29DE6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0E3B64-8FFF-430D-A2EB-A1A771A45C34}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="d198314b-e946-45aa-aae0-63b36c0ef231"/>
-    <ds:schemaRef ds:uri="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77130A33-8B41-4C6E-9374-3F37E025C758}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1240,4 +1259,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB91C2F2-1F90-48E4-A244-DEC454B29DE6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0E3B64-8FFF-430D-A2EB-A1A771A45C34}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="d198314b-e946-45aa-aae0-63b36c0ef231"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Remove personal info from SD Excel template
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
+++ b/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap-my.sharepoint.com/personal/jim_grimm_sap_com/Documents/CALM/Excel FIles/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{7886D2DD-3B43-224E-ACA0-FC38A28ED4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7E73797-A225-4044-AF26-7FB0D44BA406}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ED02A5-30F4-7942-ABD8-F4EAB0C34C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="1860" windowWidth="34560" windowHeight="19980" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="1" r:id="rId1"/>
@@ -323,10 +318,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -968,6 +959,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BC4424C304B0C84BABB48D23FBFE0C27" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5926b03e82728d2d86cd579cef044969">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d" xmlns:ns3="d198314b-e946-45aa-aae0-63b36c0ef231" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b34dfbe06df4f742cab700692c9905" ns2:_="" ns3:_="">
     <xsd:import namespace="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
@@ -1222,15 +1222,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1243,6 +1234,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB91C2F2-1F90-48E4-A244-DEC454B29DE6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77130A33-8B41-4C6E-9374-3F37E025C758}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1261,14 +1260,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB91C2F2-1F90-48E4-A244-DEC454B29DE6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0E3B64-8FFF-430D-A2EB-A1A771A45C34}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Add Responsible to Documents Template
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
+++ b/spreadsheet-examples/spreadsheet-documents/SAP Cloud ALM - Documents template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ED02A5-30F4-7942-ABD8-F4EAB0C34C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE362BCF-500F-5C43-986C-C20CF1D60153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
+    <workbookView xWindow="5640" yWindow="2120" windowWidth="51200" windowHeight="28800" xr2:uid="{8F915268-DAB3-9744-889D-7D8C75EAE1B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>Title</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>john.doe@sap.com</t>
+  </si>
+  <si>
+    <t>Responsible</t>
   </si>
 </sst>
 </file>
@@ -617,7 +620,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C19546E-5C87-714C-86D6-A993F68C66C3}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -629,12 +632,12 @@
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
-    <col min="6" max="6" width="44" customWidth="1"/>
-    <col min="7" max="7" width="64" customWidth="1"/>
+    <col min="5" max="6" width="18.1640625" customWidth="1"/>
+    <col min="7" max="7" width="44" customWidth="1"/>
+    <col min="8" max="8" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -651,13 +654,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -673,14 +679,17 @@
       <c r="E2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -696,10 +705,13 @@
       <c r="E3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -707,6 +719,8 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{AD3020AE-47DB-104F-816E-B4B1CA52C568}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{045126C1-4C00-8144-814E-AFE3FC56189A}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{FFE9D46E-D350-FB4D-9AD0-2ECBF5C709F9}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{04E97F19-EE63-F64A-8FC4-6B2A36EBBF54}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -968,6 +982,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d198314b-e946-45aa-aae0-63b36c0ef231" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BC4424C304B0C84BABB48D23FBFE0C27" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5926b03e82728d2d86cd579cef044969">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d" xmlns:ns3="d198314b-e946-45aa-aae0-63b36c0ef231" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b34dfbe06df4f742cab700692c9905" ns2:_="" ns3:_="">
     <xsd:import namespace="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
@@ -1222,17 +1247,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d198314b-e946-45aa-aae0-63b36c0ef231" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB91C2F2-1F90-48E4-A244-DEC454B29DE6}">
   <ds:schemaRefs>
@@ -1242,6 +1256,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0E3B64-8FFF-430D-A2EB-A1A771A45C34}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="d198314b-e946-45aa-aae0-63b36c0ef231"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77130A33-8B41-4C6E-9374-3F37E025C758}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1258,21 +1289,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0E3B64-8FFF-430D-A2EB-A1A771A45C34}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="d198314b-e946-45aa-aae0-63b36c0ef231"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="16a5fbcf-eb1b-4537-978b-0aed4a0d2a8d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>